<commit_message>
añadidos ejercicios 7 de noviembre
</commit_message>
<xml_diff>
--- a/m1/unidad3/Practicas/20191106/excel-11-lista-productos.xlsx
+++ b/m1/unidad3/Practicas/20191106/excel-11-lista-productos.xlsx
@@ -18,13 +18,13 @@
     <sheet name="Filtros varios" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Filtros varios'!$L$4:$N$5</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Filtros varios'!$A$111:$D$114</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Listado de Productos'!$A$3:$J$80</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Productos ordenados'!$A$3:$J$80</definedName>
-    <definedName name="_xlnm.Extract" localSheetId="3">'Filtros varios'!$A$29:$D$29</definedName>
+    <definedName name="_xlnm.Extract" localSheetId="3">'Filtros varios'!$A$122:$B$122</definedName>
     <definedName name="_xlnm.Extract" localSheetId="1">'Productos ordenados'!#REF!</definedName>
     <definedName name="_xlnm.Extract" localSheetId="2">'Productos reducidos'!$A$3:$E$3</definedName>
-    <definedName name="_xlnm.Criteria" localSheetId="3">'Filtros varios'!$A$25:$B$26</definedName>
+    <definedName name="_xlnm.Criteria" localSheetId="3">'Filtros varios'!$A$119:$A$120</definedName>
     <definedName name="_xlnm.Criteria" localSheetId="1">'Productos ordenados'!$A$85:$E$88</definedName>
     <definedName name="ejemplo_access" localSheetId="0">'Listado de Productos'!$A$3:$J$80</definedName>
     <definedName name="ejemplo_access" localSheetId="1">'Productos ordenados'!$A$3:$J$80</definedName>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="743" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="891" uniqueCount="208">
   <si>
     <t>IdProducto</t>
   </si>
@@ -650,6 +650,27 @@
   </si>
   <si>
     <t>Carnes, condimentos y lácteos</t>
+  </si>
+  <si>
+    <t>Productos que comienzan por "Cerveza"</t>
+  </si>
+  <si>
+    <t>Cerveza*</t>
+  </si>
+  <si>
+    <t>Quesos</t>
+  </si>
+  <si>
+    <t>*ueso*</t>
+  </si>
+  <si>
+    <t>*paq*</t>
+  </si>
+  <si>
+    <t>Dos proveedores</t>
+  </si>
+  <si>
+    <t>Productos suspendidos</t>
   </si>
 </sst>
 </file>
@@ -731,11 +752,11 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -790,7 +811,7 @@
       <queryTableField id="9" name="NivelNuevoPedido"/>
       <queryTableField id="10" name="Suspendido"/>
     </queryTableFields>
-    <sortState ref="A4:J80">
+    <sortState ref="A5:J80">
       <sortCondition ref="D4:D80"/>
       <sortCondition descending="1" ref="F4:F80"/>
     </sortState>
@@ -1063,8 +1084,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:J80"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="D59" sqref="D59"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3589,7 +3610,7 @@
   <dimension ref="A3:J88"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="D59" sqref="D59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6313,10 +6334,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N82"/>
+  <dimension ref="A1:N130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E43" sqref="E43"/>
+    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="C61" sqref="C61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6325,22 +6346,23 @@
     <col min="2" max="2" width="31.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
     </row>
     <row r="3" spans="1:14" ht="18" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="6" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>4</v>
       </c>
       <c r="L4" s="4"/>
@@ -6356,18 +6378,18 @@
       <c r="N5" s="4"/>
     </row>
     <row r="7" spans="1:14" ht="18" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="6" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="5" t="s">
         <v>193</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="5" t="s">
         <v>4</v>
       </c>
     </row>
@@ -6514,22 +6536,22 @@
       </c>
     </row>
     <row r="22" spans="1:6" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A22" s="5" t="s">
+      <c r="A22" s="7" t="s">
         <v>198</v>
       </c>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
     </row>
     <row r="24" spans="1:6" ht="18" x14ac:dyDescent="0.25">
-      <c r="A24" s="7" t="s">
+      <c r="A24" s="6" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="6" t="s">
+      <c r="A25" s="5" t="s">
         <v>192</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="B25" s="5" t="s">
         <v>3</v>
       </c>
     </row>
@@ -6542,21 +6564,21 @@
       </c>
     </row>
     <row r="28" spans="1:6" ht="18" x14ac:dyDescent="0.25">
-      <c r="A28" s="7" t="s">
+      <c r="A28" s="6" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A29" s="6" t="s">
+      <c r="A29" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="6" t="s">
+      <c r="B29" s="5" t="s">
         <v>193</v>
       </c>
-      <c r="C29" s="6" t="s">
+      <c r="C29" s="5" t="s">
         <v>192</v>
       </c>
-      <c r="D29" s="6" t="s">
+      <c r="D29" s="5" t="s">
         <v>3</v>
       </c>
     </row>
@@ -6662,27 +6684,27 @@
       <c r="D37" s="1"/>
     </row>
     <row r="38" spans="1:4" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A38" s="5" t="s">
+      <c r="A38" s="7" t="s">
         <v>200</v>
       </c>
-      <c r="B38" s="5"/>
-      <c r="C38" s="5"/>
+      <c r="B38" s="7"/>
+      <c r="C38" s="7"/>
       <c r="D38" s="1"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D39" s="1"/>
     </row>
     <row r="40" spans="1:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="A40" s="7" t="s">
+      <c r="A40" s="6" t="s">
         <v>195</v>
       </c>
       <c r="D40" s="1"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A41" s="6" t="s">
+      <c r="A41" s="5" t="s">
         <v>192</v>
       </c>
-      <c r="B41" s="6" t="s">
+      <c r="B41" s="5" t="s">
         <v>7</v>
       </c>
       <c r="D41" s="1"/>
@@ -6712,130 +6734,761 @@
       <c r="D45" s="1"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A46" s="6" t="s">
+      <c r="A46" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B46" s="6" t="s">
+      <c r="B46" s="5" t="s">
         <v>192</v>
       </c>
       <c r="D46" s="1"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>120</v>
+      </c>
+      <c r="B47" t="s">
+        <v>15</v>
+      </c>
       <c r="D47" s="1"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>159</v>
+      </c>
+      <c r="B48" t="s">
+        <v>39</v>
+      </c>
       <c r="D48" s="1"/>
     </row>
-    <row r="49" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>181</v>
+      </c>
+      <c r="B49" t="s">
+        <v>39</v>
+      </c>
       <c r="D49" s="1"/>
     </row>
-    <row r="50" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>144</v>
+      </c>
+      <c r="B50" t="s">
+        <v>32</v>
+      </c>
       <c r="D50" s="1"/>
     </row>
-    <row r="51" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>17</v>
+      </c>
+      <c r="B51" t="s">
+        <v>15</v>
+      </c>
       <c r="D51" s="1"/>
     </row>
-    <row r="52" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>172</v>
+      </c>
+      <c r="B52" t="s">
+        <v>15</v>
+      </c>
       <c r="D52" s="1"/>
     </row>
-    <row r="53" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>22</v>
+      </c>
+      <c r="B53" t="s">
+        <v>15</v>
+      </c>
       <c r="D53" s="1"/>
     </row>
-    <row r="54" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>20</v>
+      </c>
+      <c r="B54" t="s">
+        <v>15</v>
+      </c>
       <c r="D54" s="1"/>
     </row>
-    <row r="55" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>147</v>
+      </c>
+      <c r="B55" t="s">
+        <v>32</v>
+      </c>
       <c r="D55" s="1"/>
     </row>
-    <row r="56" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>37</v>
+      </c>
+      <c r="B56" t="s">
+        <v>39</v>
+      </c>
       <c r="D56" s="1"/>
     </row>
-    <row r="57" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>94</v>
+      </c>
+      <c r="B57" t="s">
+        <v>39</v>
+      </c>
       <c r="D57" s="1"/>
     </row>
-    <row r="58" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>89</v>
+      </c>
+      <c r="B58" t="s">
+        <v>39</v>
+      </c>
       <c r="D58" s="1"/>
     </row>
-    <row r="59" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>177</v>
+      </c>
+      <c r="B59" t="s">
+        <v>39</v>
+      </c>
       <c r="D59" s="1"/>
     </row>
-    <row r="60" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>41</v>
+      </c>
+      <c r="B60" t="s">
+        <v>39</v>
+      </c>
       <c r="D60" s="1"/>
     </row>
-    <row r="61" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>92</v>
+      </c>
+      <c r="B61" t="s">
+        <v>39</v>
+      </c>
       <c r="D61" s="1"/>
     </row>
-    <row r="62" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>182</v>
+      </c>
+      <c r="B62" t="s">
+        <v>39</v>
+      </c>
       <c r="D62" s="1"/>
     </row>
-    <row r="63" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>156</v>
+      </c>
+      <c r="B63" t="s">
+        <v>39</v>
+      </c>
       <c r="D63" s="1"/>
     </row>
-    <row r="64" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>28</v>
+      </c>
+      <c r="B64" t="s">
+        <v>15</v>
+      </c>
       <c r="D64" s="1"/>
     </row>
-    <row r="65" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>170</v>
+      </c>
+      <c r="B65" t="s">
+        <v>15</v>
+      </c>
       <c r="D65" s="1"/>
     </row>
-    <row r="66" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>48</v>
+      </c>
+      <c r="B66" t="s">
+        <v>15</v>
+      </c>
       <c r="D66" s="1"/>
     </row>
-    <row r="67" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>190</v>
+      </c>
+      <c r="B67" t="s">
+        <v>15</v>
+      </c>
       <c r="D67" s="1"/>
     </row>
-    <row r="68" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>166</v>
+      </c>
+      <c r="B68" t="s">
+        <v>15</v>
+      </c>
       <c r="D68" s="1"/>
     </row>
-    <row r="69" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>161</v>
+      </c>
+      <c r="B69" t="s">
+        <v>15</v>
+      </c>
       <c r="D69" s="1"/>
     </row>
-    <row r="70" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>14</v>
+      </c>
+      <c r="B70" t="s">
+        <v>15</v>
+      </c>
       <c r="D70" s="1"/>
     </row>
-    <row r="71" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D71" s="1"/>
     </row>
-    <row r="72" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:4" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="A72" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="B72" s="7"/>
+      <c r="C72" s="7"/>
       <c r="D72" s="1"/>
     </row>
-    <row r="73" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D73" s="1"/>
     </row>
-    <row r="74" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+      <c r="A74" s="6" t="s">
+        <v>195</v>
+      </c>
       <c r="D74" s="1"/>
     </row>
-    <row r="75" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A75" s="5" t="s">
+        <v>1</v>
+      </c>
       <c r="D75" s="1"/>
     </row>
-    <row r="76" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>202</v>
+      </c>
       <c r="D76" s="1"/>
     </row>
-    <row r="77" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D77" s="1"/>
     </row>
-    <row r="78" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D78" s="1"/>
-    </row>
-    <row r="79" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D79" s="1"/>
-    </row>
-    <row r="80" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D80" s="1"/>
-    </row>
-    <row r="81" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D81" s="1"/>
-    </row>
-    <row r="82" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D82" s="1"/>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A78" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B78" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C78" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="D78" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A79">
+        <v>2</v>
+      </c>
+      <c r="B79" t="s">
+        <v>12</v>
+      </c>
+      <c r="C79" t="s">
+        <v>9</v>
+      </c>
+      <c r="D79" s="1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A80">
+        <v>34</v>
+      </c>
+      <c r="B80" t="s">
+        <v>97</v>
+      </c>
+      <c r="C80" t="s">
+        <v>98</v>
+      </c>
+      <c r="D80" s="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A81">
+        <v>35</v>
+      </c>
+      <c r="B81" t="s">
+        <v>99</v>
+      </c>
+      <c r="C81" t="s">
+        <v>98</v>
+      </c>
+      <c r="D81" s="1">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A82">
+        <v>67</v>
+      </c>
+      <c r="B82" t="s">
+        <v>174</v>
+      </c>
+      <c r="C82" t="s">
+        <v>98</v>
+      </c>
+      <c r="D82" s="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A83">
+        <v>70</v>
+      </c>
+      <c r="B83" t="s">
+        <v>179</v>
+      </c>
+      <c r="C83" t="s">
+        <v>51</v>
+      </c>
+      <c r="D83" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A84">
+        <v>75</v>
+      </c>
+      <c r="B84" t="s">
+        <v>186</v>
+      </c>
+      <c r="C84" t="s">
+        <v>82</v>
+      </c>
+      <c r="D84" s="1">
+        <v>7.75</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="A86" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="B86" s="7"/>
+      <c r="C86" s="7"/>
+    </row>
+    <row r="88" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="A88" s="6" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A89" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B89" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>204</v>
+      </c>
+      <c r="B90" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A93" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B93" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C93" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="D93" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E93" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A94">
+        <v>74</v>
+      </c>
+      <c r="B94" t="s">
+        <v>185</v>
+      </c>
+      <c r="C94" t="s">
+        <v>31</v>
+      </c>
+      <c r="D94" s="1">
+        <v>10</v>
+      </c>
+      <c r="E94" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A95">
+        <v>31</v>
+      </c>
+      <c r="B95" t="s">
+        <v>89</v>
+      </c>
+      <c r="C95" t="s">
+        <v>90</v>
+      </c>
+      <c r="D95" s="1">
+        <v>12.5</v>
+      </c>
+      <c r="E95" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A96">
+        <v>11</v>
+      </c>
+      <c r="B96" t="s">
+        <v>37</v>
+      </c>
+      <c r="C96" t="s">
+        <v>38</v>
+      </c>
+      <c r="D96" s="1">
+        <v>21</v>
+      </c>
+      <c r="E96" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A97">
+        <v>71</v>
+      </c>
+      <c r="B97" t="s">
+        <v>181</v>
+      </c>
+      <c r="C97" t="s">
+        <v>95</v>
+      </c>
+      <c r="D97" s="1">
+        <v>21.5</v>
+      </c>
+      <c r="E97" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A98">
+        <v>32</v>
+      </c>
+      <c r="B98" t="s">
+        <v>92</v>
+      </c>
+      <c r="C98" t="s">
+        <v>90</v>
+      </c>
+      <c r="D98" s="1">
+        <v>32</v>
+      </c>
+      <c r="E98" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A99">
+        <v>72</v>
+      </c>
+      <c r="B99" t="s">
+        <v>182</v>
+      </c>
+      <c r="C99" t="s">
+        <v>90</v>
+      </c>
+      <c r="D99" s="1">
+        <v>34.799999999999997</v>
+      </c>
+      <c r="E99" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A100">
+        <v>69</v>
+      </c>
+      <c r="B100" t="s">
+        <v>177</v>
+      </c>
+      <c r="C100" t="s">
+        <v>95</v>
+      </c>
+      <c r="D100" s="1">
+        <v>36</v>
+      </c>
+      <c r="E100" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A101">
+        <v>12</v>
+      </c>
+      <c r="B101" t="s">
+        <v>41</v>
+      </c>
+      <c r="C101" t="s">
+        <v>38</v>
+      </c>
+      <c r="D101" s="1">
+        <v>38</v>
+      </c>
+      <c r="E101" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A102">
+        <v>59</v>
+      </c>
+      <c r="B102" t="s">
+        <v>156</v>
+      </c>
+      <c r="C102" t="s">
+        <v>157</v>
+      </c>
+      <c r="D102" s="1">
+        <v>55</v>
+      </c>
+      <c r="E102" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="A104" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="B104" s="7"/>
+      <c r="C104" s="7"/>
+    </row>
+    <row r="106" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="A106" s="6" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A107" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="B107" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="C107" s="5"/>
+      <c r="D107" s="5"/>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
+        <v>9</v>
+      </c>
+      <c r="B108" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
+        <v>116</v>
+      </c>
+      <c r="B109" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A111" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B111" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="C111" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="D111" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A112" t="s">
+        <v>12</v>
+      </c>
+      <c r="B112" t="s">
+        <v>9</v>
+      </c>
+      <c r="C112" t="s">
+        <v>10</v>
+      </c>
+      <c r="D112" s="1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A113" t="s">
+        <v>8</v>
+      </c>
+      <c r="B113" t="s">
+        <v>9</v>
+      </c>
+      <c r="C113" t="s">
+        <v>10</v>
+      </c>
+      <c r="D113" s="1">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A114" t="s">
+        <v>120</v>
+      </c>
+      <c r="B114" t="s">
+        <v>116</v>
+      </c>
+      <c r="C114" t="s">
+        <v>15</v>
+      </c>
+      <c r="D114" s="1">
+        <v>19.45</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="A116" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="B116" s="7"/>
+      <c r="C116" s="7"/>
+    </row>
+    <row r="118" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+      <c r="A118" s="6" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A119" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A120" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A122" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B122" s="5" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A123" t="s">
+        <v>142</v>
+      </c>
+      <c r="B123" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A124" t="s">
+        <v>115</v>
+      </c>
+      <c r="B124" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A125" t="s">
+        <v>20</v>
+      </c>
+      <c r="B125" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A126" t="s">
+        <v>54</v>
+      </c>
+      <c r="B126" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A127" t="s">
+        <v>84</v>
+      </c>
+      <c r="B127" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A128" t="s">
+        <v>81</v>
+      </c>
+      <c r="B128" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A129" t="s">
+        <v>71</v>
+      </c>
+      <c r="B129" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A130" t="s">
+        <v>30</v>
+      </c>
+      <c r="B130" t="s">
+        <v>31</v>
+      </c>
     </row>
   </sheetData>
-  <sortState ref="A30:D36">
-    <sortCondition descending="1" ref="D30:D36"/>
+  <sortState ref="A123:B130">
+    <sortCondition ref="B123:B130"/>
   </sortState>
-  <mergeCells count="3">
+  <mergeCells count="7">
+    <mergeCell ref="A104:C104"/>
+    <mergeCell ref="A116:C116"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A22:C22"/>
     <mergeCell ref="A38:C38"/>
+    <mergeCell ref="A72:C72"/>
+    <mergeCell ref="A86:C86"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>